<commit_message>
add temperature and rainfall 2
</commit_message>
<xml_diff>
--- a/data/macroeconomic/economic_activity.xlsx
+++ b/data/macroeconomic/economic_activity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\time_series_padova\data\macroeconomic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFC530B-09D0-4F98-BA29-93FE3FB525B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1C82C6-DDB4-4FF3-963D-08D2CE5D8126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E59D194-54AD-4097-BBAD-40E9B6DCEB8A}"/>
   </bookViews>
@@ -96,9 +96,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -438,7 +438,7 @@
   <dimension ref="A1:B237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>